<commit_message>
Adding in starter code to get MHOR estimates
</commit_message>
<xml_diff>
--- a/cmh/Results/R/R_3HA_vcdExtra_forked.xlsx
+++ b/cmh/Results/R/R_3HA_vcdExtra_forked.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="51">
   <si>
     <t>Schema</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>Prob</t>
+  </si>
+  <si>
+    <t>results</t>
   </si>
   <si>
     <t>1</t>
@@ -229,345 +232,399 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="G2" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="G3" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="G4" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="G7" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="G11" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="G12" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="G13" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="G15" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="G16" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="G17" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding SAS-based CMH Results
</commit_message>
<xml_diff>
--- a/cmh/Results/R/R_3HA_vcdExtra_forked.xlsx
+++ b/cmh/Results/R/R_3HA_vcdExtra_forked.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
   <si>
     <t>Schema</t>
   </si>
@@ -83,6 +83,15 @@
     <t>17</t>
   </si>
   <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>General Association</t>
   </si>
   <si>
@@ -113,6 +122,9 @@
     <t>0.00101244204262285</t>
   </si>
   <si>
+    <t>NaN</t>
+  </si>
+  <si>
     <t>NULL</t>
   </si>
   <si>
@@ -125,13 +137,13 @@
     <t>0.0076021635258659</t>
   </si>
   <si>
-    <t>7.62641901466917</t>
-  </si>
-  <si>
-    <t>3.45670566179605</t>
-  </si>
-  <si>
-    <t>0.0940833712213925</t>
+    <t>5.73053819338041</t>
+  </si>
+  <si>
+    <t>3.04452700866735</t>
+  </si>
+  <si>
+    <t>0.871529542290134</t>
   </si>
   <si>
     <t>0.894248695441543</t>
@@ -158,13 +170,13 @@
     <t>0.930520180590414</t>
   </si>
   <si>
-    <t>0.00575193950235399</t>
-  </si>
-  <si>
-    <t>0.177576668005366</t>
-  </si>
-  <si>
-    <t>0.999999803487966</t>
+    <t>0.0166723722968053</t>
+  </si>
+  <si>
+    <t>0.5504017626057</t>
+  </si>
+  <si>
+    <t>0.998937021911653</t>
   </si>
 </sst>
 </file>
@@ -244,16 +256,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G2" t="e">
         <v>#N/A</v>
@@ -267,16 +279,16 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G3" t="e">
         <v>#N/A</v>
@@ -290,16 +302,16 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G4" t="e">
         <v>#N/A</v>
@@ -313,16 +325,16 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G5" t="e">
         <v>#N/A</v>
@@ -336,16 +348,16 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G6" t="e">
         <v>#N/A</v>
@@ -359,16 +371,16 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G7" t="e">
         <v>#N/A</v>
@@ -385,16 +397,16 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="G8" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="9">
@@ -402,22 +414,22 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="10">
@@ -425,22 +437,22 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="G10" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="11">
@@ -448,22 +460,22 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="e">
-        <v>#N/A</v>
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12">
@@ -471,22 +483,22 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" t="e">
-        <v>#N/A</v>
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13">
@@ -497,16 +509,16 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G13" t="e">
         <v>#N/A</v>
@@ -517,22 +529,22 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>26</v>
+        <v>50</v>
+      </c>
+      <c r="G14" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="15">
@@ -540,19 +552,19 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G15" t="e">
         <v>#N/A</v>
@@ -563,22 +575,22 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" t="e">
-        <v>#N/A</v>
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17">
@@ -589,19 +601,19 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" t="e">
-        <v>#N/A</v>
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18">
@@ -612,19 +624,88 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" t="s">
-        <v>26</v>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>